<commit_message>
Hoàn thiện Dynamic Action list top
</commit_message>
<xml_diff>
--- a/wwwroot/AttachmentFiles/FILETEMPLATEREPORT/20250326/Nhập booking template_202503263801.xlsx
+++ b/wwwroot/AttachmentFiles/FILETEMPLATEREPORT/20250326/Nhập booking template_202503263801.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\KOA Home\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\ASP.Net project\KOA Home ASP.NET Core\wwwroot\AttachmentFiles\FILETEMPLATEREPORT\20250326\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8ECC2C-DEBB-47AF-8F33-1B013817598D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF796554-14C4-44BD-BF25-F4B8858ED2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" xr2:uid="{3AA19672-7DFE-434F-8451-7F4AA595ECEA}"/>
   </bookViews>
@@ -144,10 +144,10 @@
     <t>Mẫu nhập dữ liệu</t>
   </si>
   <si>
-    <t>HS_Booking_Import</t>
+    <t>Thông tin nhập (tham khảo mẫu nhập)</t>
   </si>
   <si>
-    <t>Thông tin nhập (tham khảo mẫu nhập)</t>
+    <t>HS_Booking_Json_Import</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="29" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -4194,15 +4194,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A622E5-3BF7-4BAC-8BB1-E1A9D84A3EAB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>